<commit_message>
update Bao cao hoan thien
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HOCTAP\QuanTriDuAn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QuanTriDuAn\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF70C68-5D73-4C97-8175-F88CC64A5E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>STT</t>
   </si>
@@ -51,12 +61,6 @@
   </si>
   <si>
     <t>Thời gian thực hiện</t>
-  </si>
-  <si>
-    <t>Khảo sát yêu cầu dự án</t>
-  </si>
-  <si>
-    <t>Bắt đầu dự án</t>
   </si>
   <si>
     <t>Lập kế hoạch phạm vi dự án</t>
@@ -124,11 +128,23 @@
   <si>
     <t>Tháng 5</t>
   </si>
+  <si>
+    <t>Lập kế hoạch cho dự án</t>
+  </si>
+  <si>
+    <t>Gặp gỡ khách hàng, tìm hiểu yêu cầu</t>
+  </si>
+  <si>
+    <t>Phân tích, khảo sát yêu cầu dự án</t>
+  </si>
+  <si>
+    <t>Tháng 4 + 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd"/>
   </numFmts>
@@ -180,7 +196,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +206,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -324,6 +346,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -342,12 +370,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,102 +693,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AO9" sqref="AO9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" style="10" customWidth="1"/>
-    <col min="5" max="65" width="4.26953125" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="10" customWidth="1"/>
+    <col min="5" max="65" width="4.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20"/>
-      <c r="AW1" s="20"/>
-      <c r="AX1" s="20"/>
-      <c r="AY1" s="20"/>
-      <c r="AZ1" s="20"/>
-      <c r="BA1" s="20"/>
-      <c r="BB1" s="20"/>
-      <c r="BC1" s="20"/>
-      <c r="BD1" s="20"/>
-      <c r="BE1" s="20"/>
-      <c r="BF1" s="20"/>
-      <c r="BG1" s="20"/>
-      <c r="BH1" s="20"/>
-      <c r="BI1" s="20"/>
-      <c r="BJ1" s="20"/>
-      <c r="BK1" s="20"/>
-      <c r="BL1" s="20"/>
-      <c r="BM1" s="20"/>
-    </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22"/>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
@@ -956,7 +979,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1031,12 +1054,12 @@
       <c r="BL3" s="7"/>
       <c r="BM3" s="7"/>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="8">
         <v>44656</v>
@@ -1049,7 +1072,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -1106,7 +1129,7 @@
       <c r="BL4" s="7"/>
       <c r="BM4" s="7"/>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -1181,7 +1204,7 @@
       <c r="BL5" s="7"/>
       <c r="BM5" s="7"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -1256,7 +1279,7 @@
       <c r="BL6" s="7"/>
       <c r="BM6" s="7"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -1331,53 +1354,53 @@
       <c r="BL7" s="7"/>
       <c r="BM7" s="7"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
-      <c r="X11" s="22"/>
-      <c r="Y11" s="22"/>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="22"/>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="22"/>
-      <c r="AG11" s="22"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="16"/>
+      <c r="AC11" s="16"/>
+      <c r="AD11" s="16"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="16"/>
       <c r="AH11" s="3"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.35">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
@@ -1504,12 +1527,12 @@
         <v>44681</v>
       </c>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>1</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C13" s="8">
         <v>44652</v>
@@ -1548,12 +1571,12 @@
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>1.1000000000000001</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C14" s="8">
         <v>44652</v>
@@ -1592,12 +1615,12 @@
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>1.2</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C15" s="8">
         <v>44653</v>
@@ -1636,18 +1659,18 @@
       <c r="AG15" s="7"/>
       <c r="AH15" s="7"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>1.3</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" s="8">
         <v>44654</v>
       </c>
       <c r="D16" s="8">
-        <v>44655</v>
+        <v>44656</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1680,18 +1703,18 @@
       <c r="AG16" s="7"/>
       <c r="AH16" s="7"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>1.4</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17" s="8">
         <v>44656</v>
       </c>
       <c r="D17" s="8">
-        <v>44656</v>
+        <v>44657</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -1724,53 +1747,53 @@
       <c r="AG17" s="7"/>
       <c r="AH17" s="7"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22"/>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="22"/>
-      <c r="AB20" s="22"/>
-      <c r="AC20" s="22"/>
-      <c r="AD20" s="22"/>
-      <c r="AE20" s="22"/>
-      <c r="AF20" s="22"/>
-      <c r="AG20" s="22"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="16"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="16"/>
+      <c r="AB20" s="16"/>
+      <c r="AC20" s="16"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="16"/>
+      <c r="AF20" s="16"/>
+      <c r="AG20" s="16"/>
       <c r="AH20" s="3"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="9" t="s">
         <v>6</v>
       </c>
@@ -1897,18 +1920,18 @@
         <v>44681</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>2</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" s="8">
-        <v>44656</v>
+        <v>44657</v>
       </c>
       <c r="D22" s="8">
-        <v>44681</v>
+        <v>44675</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1941,18 +1964,18 @@
       <c r="AG22" s="7"/>
       <c r="AH22" s="7"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>2.1</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" s="8">
-        <v>44656</v>
+        <v>44657</v>
       </c>
       <c r="D23" s="8">
-        <v>44660</v>
+        <v>44662</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1985,15 +2008,15 @@
       <c r="AG23" s="7"/>
       <c r="AH23" s="7"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>2.2000000000000002</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C24" s="8">
-        <v>44661</v>
+        <v>44662</v>
       </c>
       <c r="D24" s="8">
         <v>44666</v>
@@ -2029,18 +2052,18 @@
       <c r="AG24" s="7"/>
       <c r="AH24" s="7"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>2.2999999999999998</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C25" s="8">
         <v>44667</v>
       </c>
       <c r="D25" s="8">
-        <v>44669</v>
+        <v>44676</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -2073,18 +2096,18 @@
       <c r="AG25" s="7"/>
       <c r="AH25" s="7"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>2.4</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C26" s="8">
-        <v>44670</v>
+        <v>44676</v>
       </c>
       <c r="D26" s="8">
-        <v>44680</v>
+        <v>44677</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -2117,18 +2140,18 @@
       <c r="AG26" s="7"/>
       <c r="AH26" s="7"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>2.5</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C27" s="8">
-        <v>44681</v>
+        <v>44676</v>
       </c>
       <c r="D27" s="8">
-        <v>44681</v>
+        <v>44677</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -2161,54 +2184,54 @@
       <c r="AG27" s="7"/>
       <c r="AH27" s="7"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A30" s="22" t="s">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="17"/>
-      <c r="V30" s="17"/>
-      <c r="W30" s="17"/>
-      <c r="X30" s="17"/>
-      <c r="Y30" s="17"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="17"/>
-      <c r="AB30" s="17"/>
-      <c r="AC30" s="17"/>
-      <c r="AD30" s="17"/>
-      <c r="AE30" s="17"/>
-      <c r="AF30" s="17"/>
-      <c r="AG30" s="17"/>
-      <c r="AH30" s="17"/>
-      <c r="AI30" s="18"/>
-    </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="19"/>
+      <c r="Y30" s="19"/>
+      <c r="Z30" s="19"/>
+      <c r="AA30" s="19"/>
+      <c r="AB30" s="19"/>
+      <c r="AC30" s="19"/>
+      <c r="AD30" s="19"/>
+      <c r="AE30" s="19"/>
+      <c r="AF30" s="19"/>
+      <c r="AG30" s="19"/>
+      <c r="AH30" s="19"/>
+      <c r="AI30" s="20"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="15" t="s">
         <v>6</v>
       </c>
@@ -2309,7 +2332,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>3</v>
       </c>
@@ -2320,7 +2343,7 @@
         <v>44682</v>
       </c>
       <c r="D32" s="8">
-        <v>44701</v>
+        <v>44707</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -2354,12 +2377,12 @@
       <c r="AH32" s="7"/>
       <c r="AI32" s="7"/>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>3.1</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C33" s="8">
         <v>44682</v>
@@ -2399,12 +2422,12 @@
       <c r="AH33" s="7"/>
       <c r="AI33" s="7"/>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>3.2</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C34" s="8">
         <v>44685</v>
@@ -2444,12 +2467,12 @@
       <c r="AH34" s="7"/>
       <c r="AI34" s="7"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>3.3</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C35" s="8">
         <v>44688</v>
@@ -2489,12 +2512,12 @@
       <c r="AH35" s="7"/>
       <c r="AI35" s="7"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>3.4</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C36" s="8">
         <v>44698</v>
@@ -2534,12 +2557,12 @@
       <c r="AH36" s="7"/>
       <c r="AI36" s="7"/>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>3.5</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C37" s="8">
         <v>44700</v>
@@ -2579,12 +2602,12 @@
       <c r="AH37" s="7"/>
       <c r="AI37" s="7"/>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>3.6</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C38" s="8">
         <v>44701</v>
@@ -2624,54 +2647,54 @@
       <c r="AH38" s="7"/>
       <c r="AI38" s="7"/>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A41" s="22" t="s">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A41" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="17"/>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
-      <c r="Q41" s="17"/>
-      <c r="R41" s="17"/>
-      <c r="S41" s="17"/>
-      <c r="T41" s="17"/>
-      <c r="U41" s="17"/>
-      <c r="V41" s="17"/>
-      <c r="W41" s="17"/>
-      <c r="X41" s="17"/>
-      <c r="Y41" s="17"/>
-      <c r="Z41" s="17"/>
-      <c r="AA41" s="17"/>
-      <c r="AB41" s="17"/>
-      <c r="AC41" s="17"/>
-      <c r="AD41" s="17"/>
-      <c r="AE41" s="17"/>
-      <c r="AF41" s="17"/>
-      <c r="AG41" s="17"/>
-      <c r="AH41" s="17"/>
-      <c r="AI41" s="18"/>
-    </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A42" s="22"/>
-      <c r="B42" s="23"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="19"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="19"/>
+      <c r="Y41" s="19"/>
+      <c r="Z41" s="19"/>
+      <c r="AA41" s="19"/>
+      <c r="AB41" s="19"/>
+      <c r="AC41" s="19"/>
+      <c r="AD41" s="19"/>
+      <c r="AE41" s="19"/>
+      <c r="AF41" s="19"/>
+      <c r="AG41" s="19"/>
+      <c r="AH41" s="19"/>
+      <c r="AI41" s="20"/>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A42" s="16"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="9" t="s">
         <v>6</v>
       </c>
@@ -2802,7 +2825,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>4</v>
       </c>
@@ -2847,12 +2870,12 @@
       <c r="AH43" s="7"/>
       <c r="AI43" s="7"/>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>4.0999999999999996</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C44" s="8">
         <v>44702</v>
@@ -2892,12 +2915,12 @@
       <c r="AH44" s="7"/>
       <c r="AI44" s="7"/>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>4.2</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C45" s="8">
         <v>44703</v>
@@ -2937,12 +2960,12 @@
       <c r="AH45" s="7"/>
       <c r="AI45" s="7"/>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>4.3</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C46" s="8">
         <v>44705</v>
@@ -2982,54 +3005,54 @@
       <c r="AH46" s="7"/>
       <c r="AI46" s="7"/>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A49" s="22" t="s">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A49" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="17"/>
-      <c r="K49" s="17"/>
-      <c r="L49" s="17"/>
-      <c r="M49" s="17"/>
-      <c r="N49" s="17"/>
-      <c r="O49" s="17"/>
-      <c r="P49" s="17"/>
-      <c r="Q49" s="17"/>
-      <c r="R49" s="17"/>
-      <c r="S49" s="17"/>
-      <c r="T49" s="17"/>
-      <c r="U49" s="17"/>
-      <c r="V49" s="17"/>
-      <c r="W49" s="17"/>
-      <c r="X49" s="17"/>
-      <c r="Y49" s="17"/>
-      <c r="Z49" s="17"/>
-      <c r="AA49" s="17"/>
-      <c r="AB49" s="17"/>
-      <c r="AC49" s="17"/>
-      <c r="AD49" s="17"/>
-      <c r="AE49" s="17"/>
-      <c r="AF49" s="17"/>
-      <c r="AG49" s="17"/>
-      <c r="AH49" s="17"/>
-      <c r="AI49" s="18"/>
-    </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A50" s="22"/>
-      <c r="B50" s="23"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="O49" s="19"/>
+      <c r="P49" s="19"/>
+      <c r="Q49" s="19"/>
+      <c r="R49" s="19"/>
+      <c r="S49" s="19"/>
+      <c r="T49" s="19"/>
+      <c r="U49" s="19"/>
+      <c r="V49" s="19"/>
+      <c r="W49" s="19"/>
+      <c r="X49" s="19"/>
+      <c r="Y49" s="19"/>
+      <c r="Z49" s="19"/>
+      <c r="AA49" s="19"/>
+      <c r="AB49" s="19"/>
+      <c r="AC49" s="19"/>
+      <c r="AD49" s="19"/>
+      <c r="AE49" s="19"/>
+      <c r="AF49" s="19"/>
+      <c r="AG49" s="19"/>
+      <c r="AH49" s="19"/>
+      <c r="AI49" s="20"/>
+    </row>
+    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A50" s="16"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="9" t="s">
         <v>6</v>
       </c>
@@ -3160,7 +3183,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>5</v>
       </c>
@@ -3205,12 +3228,12 @@
       <c r="AH51" s="7"/>
       <c r="AI51" s="7"/>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>5.0999999999999996</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C52" s="8">
         <v>44708</v>
@@ -3250,12 +3273,12 @@
       <c r="AH52" s="7"/>
       <c r="AI52" s="7"/>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>5.2</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C53" s="8">
         <v>44709</v>
@@ -3295,12 +3318,12 @@
       <c r="AH53" s="7"/>
       <c r="AI53" s="7"/>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>5.3</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C54" s="8">
         <v>44711</v>
@@ -3342,16 +3365,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="E11:AG11"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E41:AI41"/>
     <mergeCell ref="E49:AI49"/>
     <mergeCell ref="E1:AH1"/>
     <mergeCell ref="AI1:BM1"/>
@@ -3367,6 +3380,16 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E11:AG11"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E41:AI41"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:BM7">
     <cfRule type="expression" dxfId="5" priority="7">

</xml_diff>